<commit_message>
Updated some more in the artifacts file
</commit_message>
<xml_diff>
--- a/doc/_editable/Artifacts.xlsx
+++ b/doc/_editable/Artifacts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\WYSIWYD\doc\_editable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="MyBar Artifacts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'MyBar Artifacts'!$A$1:$E$56</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'MyBar Artifacts'!$A$1:$E$60</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="126">
   <si>
     <t>Notes</t>
   </si>
@@ -336,9 +336,6 @@
     <t>Dag Fridén, Mathias Bjurbäck</t>
   </si>
   <si>
-    <t>We tried this the first half of the project to set up meetings et cetera</t>
-  </si>
-  <si>
     <t>Mailflow (Production)</t>
   </si>
   <si>
@@ -382,13 +379,34 @@
   </si>
   <si>
     <t>Mostly with robotium</t>
+  </si>
+  <si>
+    <t>Sunday Meeting Notes and Chairman</t>
+  </si>
+  <si>
+    <t>GitHub (Preparation and Installation)</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>Logics</t>
+  </si>
+  <si>
+    <t>Dag Fridén, Mathias Karlgren</t>
+  </si>
+  <si>
+    <t>We tried to use SharePoint the first half of the project, to set up meetings et cetera</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -441,6 +459,11 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -524,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -552,12 +575,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -584,6 +601,18 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -643,7 +672,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -667,7 +696,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -891,14 +920,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F104" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A2:F104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F110" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F110"/>
   <tableColumns count="6">
     <tableColumn id="1" name="General Context" dataDxfId="5"/>
     <tableColumn id="2" name="Particular Context" dataDxfId="4"/>
     <tableColumn id="12" name="Main Contributors" dataDxfId="3"/>
-    <tableColumn id="3" name="Contributors" dataDxfId="1"/>
-    <tableColumn id="13" name="Notes" dataDxfId="2"/>
+    <tableColumn id="3" name="Contributors" dataDxfId="2"/>
+    <tableColumn id="13" name="Notes" dataDxfId="1"/>
     <tableColumn id="5" name="Notes 2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1194,13 +1223,13 @@
     <tabColor theme="6" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G165"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C69" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B78" sqref="B78"/>
+      <selection pane="bottomRight" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1209,16 +1238,16 @@
     <col min="2" max="2" width="33.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="66.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="67" style="4" customWidth="1"/>
+    <col min="5" max="5" width="71.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="22"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="10"/>
@@ -1226,10 +1255,10 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>41</v>
@@ -1240,13 +1269,13 @@
       <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="18" t="s">
         <v>91</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>52</v>
       </c>
       <c r="B3" s="5"/>
@@ -1257,7 +1286,7 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
@@ -1268,7 +1297,7 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1283,7 +1312,7 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1298,7 +1327,7 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1313,7 +1342,7 @@
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1330,7 +1359,7 @@
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1345,7 +1374,7 @@
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1362,7 +1391,7 @@
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1377,7 +1406,7 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1396,7 +1425,7 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1411,7 +1440,7 @@
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1426,7 +1455,7 @@
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1443,7 +1472,7 @@
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1458,7 +1487,7 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1469,13 +1498,13 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1490,7 +1519,7 @@
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1505,7 +1534,7 @@
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="5"/>
@@ -1516,7 +1545,7 @@
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1531,7 +1560,7 @@
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1546,7 +1575,7 @@
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1561,7 +1590,7 @@
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="5"/>
@@ -1572,7 +1601,7 @@
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1589,7 +1618,7 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1604,7 +1633,7 @@
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1619,7 +1648,7 @@
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1634,7 +1663,7 @@
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="5"/>
@@ -1645,7 +1674,7 @@
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1660,7 +1689,7 @@
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1675,7 +1704,7 @@
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1690,7 +1719,7 @@
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1705,7 +1734,7 @@
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1718,7 +1747,7 @@
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="5"/>
@@ -1729,7 +1758,7 @@
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -1744,7 +1773,7 @@
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="13" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="5"/>
@@ -1755,7 +1784,7 @@
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1770,7 +1799,7 @@
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -1789,13 +1818,13 @@
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="16" t="s">
         <v>57</v>
       </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B42" s="4" t="s">
@@ -1807,7 +1836,7 @@
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -1819,7 +1848,7 @@
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B44" s="4" t="s">
@@ -1834,7 +1863,7 @@
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -1846,35 +1875,35 @@
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B46" s="17" t="s">
+      <c r="A46" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="17" t="s">
+      <c r="A47" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -1886,707 +1915,773 @@
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="5"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="23"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="23"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="23"/>
+      <c r="B51" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="23"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="5"/>
+      <c r="B52" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="23"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="23"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="3"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="3"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F61" s="5"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="15"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D69" s="15"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D70" s="15"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="15"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D75" s="15"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="5"/>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E77" s="15"/>
+      <c r="F77" s="5"/>
+    </row>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="5"/>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="5"/>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C51" s="17" t="s">
+      <c r="C79" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17" t="s">
+      <c r="D79" s="15"/>
+      <c r="E79" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="15"/>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B83" s="15"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D84" s="15"/>
+      <c r="E84" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F84" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="5"/>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="3"/>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="3"/>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="17" t="s">
+      <c r="C85" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D85" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E85" s="24"/>
+      <c r="F85" s="23"/>
+    </row>
+    <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D86" s="15"/>
+      <c r="E86" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F86" s="5"/>
+    </row>
+    <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="15"/>
+      <c r="B89" s="15"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="5"/>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="15"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="15"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D91" s="15"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C93" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="23"/>
+    </row>
+    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C95" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="3"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="3"/>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B57" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="F57" s="5"/>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="17"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="5"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="5"/>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="5"/>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C61" s="17" t="s">
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C96" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="5"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="5"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="5"/>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="5"/>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="5"/>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="5"/>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="5"/>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D68" s="17"/>
-      <c r="E68" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="F68" s="5"/>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="5"/>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="5"/>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="5"/>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C72" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="5"/>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D73" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E73" s="17"/>
-      <c r="F73" s="5"/>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="5"/>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="F75" s="5"/>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="5"/>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D77" s="17"/>
-      <c r="E77" s="17"/>
-      <c r="F77" s="5"/>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="17"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="5"/>
-    </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B79" s="17"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="17"/>
-      <c r="E79" s="17"/>
-      <c r="F79" s="5"/>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C80" s="17" t="s">
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C97" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="F80" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C81" s="17" t="s">
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C98" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="F81" s="5"/>
-    </row>
-    <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="F82" s="5"/>
-    </row>
-    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D83" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E83" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="F83" s="5"/>
-    </row>
-    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="17"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="5"/>
-    </row>
-    <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B85" s="17"/>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="5"/>
-    </row>
-    <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C86" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
-      <c r="F86" s="5"/>
-    </row>
-    <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C87" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D87" s="17"/>
-      <c r="E87" s="17"/>
-      <c r="F87" s="5"/>
-    </row>
-    <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D88" s="17"/>
-      <c r="E88" s="17"/>
-      <c r="F88" s="5"/>
-    </row>
-    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
-      <c r="F89" s="5"/>
-    </row>
-    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
-      <c r="F90" s="5"/>
-    </row>
-    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91" s="17" t="s">
+      <c r="D98" s="15"/>
+      <c r="E98" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C91" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D91" s="17"/>
-      <c r="E91" s="17"/>
-      <c r="F91" s="5"/>
-    </row>
-    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B92" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C92" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D92" s="17"/>
-      <c r="E92" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F92" s="5"/>
-    </row>
-    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B93" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C93" s="17" t="s">
+      <c r="C99" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="5"/>
-    </row>
-    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="17"/>
-      <c r="B94" s="17"/>
-      <c r="C94" s="17"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="5"/>
-    </row>
-    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="17"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
-      <c r="F95" s="5"/>
-    </row>
-    <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="17"/>
-      <c r="B96" s="17"/>
-      <c r="C96" s="17"/>
-      <c r="D96" s="17"/>
-      <c r="E96" s="17"/>
-      <c r="F96" s="5"/>
-    </row>
-    <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="17"/>
-      <c r="B97" s="17"/>
-      <c r="C97" s="17"/>
-      <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
-      <c r="F97" s="5"/>
-    </row>
-    <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="17"/>
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
-      <c r="F98" s="5"/>
-    </row>
-    <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="17"/>
-      <c r="B99" s="17"/>
-      <c r="C99" s="17"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="17"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="15"/>
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="17"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="17"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="17"/>
+      <c r="A100" s="15"/>
+      <c r="B100" s="15"/>
+      <c r="C100" s="15"/>
+      <c r="D100" s="15"/>
+      <c r="E100" s="15"/>
       <c r="F100" s="5"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="17"/>
-      <c r="B101" s="17"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17"/>
+      <c r="A101" s="15"/>
+      <c r="B101" s="15"/>
+      <c r="C101" s="15"/>
+      <c r="D101" s="15"/>
+      <c r="E101" s="15"/>
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="17"/>
-      <c r="B102" s="17"/>
-      <c r="C102" s="17"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="17"/>
+      <c r="A102" s="15"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="15"/>
+      <c r="D102" s="15"/>
+      <c r="E102" s="15"/>
       <c r="F102" s="5"/>
     </row>
     <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="17"/>
-      <c r="B103" s="17"/>
-      <c r="C103" s="17"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="17"/>
+      <c r="A103" s="15"/>
+      <c r="B103" s="15"/>
+      <c r="C103" s="15"/>
+      <c r="D103" s="15"/>
+      <c r="E103" s="15"/>
       <c r="F103" s="5"/>
     </row>
     <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="17"/>
-      <c r="B104" s="17"/>
-      <c r="C104" s="17"/>
-      <c r="D104" s="17"/>
-      <c r="E104" s="17"/>
+      <c r="A104" s="15"/>
+      <c r="B104" s="15"/>
+      <c r="C104" s="15"/>
+      <c r="D104" s="15"/>
+      <c r="E104" s="15"/>
       <c r="F104" s="5"/>
     </row>
-    <row r="105" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="15"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="15"/>
+      <c r="D105" s="15"/>
+      <c r="E105" s="15"/>
+      <c r="F105" s="5"/>
+    </row>
+    <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="15"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="15"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="5"/>
+    </row>
+    <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="15"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="5"/>
+    </row>
+    <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="15"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="15"/>
+      <c r="D108" s="15"/>
+      <c r="E108" s="15"/>
+      <c r="F108" s="5"/>
+    </row>
+    <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="15"/>
+      <c r="B109" s="15"/>
+      <c r="C109" s="15"/>
+      <c r="D109" s="15"/>
+      <c r="E109" s="15"/>
+      <c r="F109" s="5"/>
+    </row>
+    <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="15"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="15"/>
+      <c r="D110" s="15"/>
+      <c r="E110" s="15"/>
+      <c r="F110" s="5"/>
+    </row>
     <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2642,6 +2737,12 @@
     <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Robotium testing document and other updates
</commit_message>
<xml_diff>
--- a/doc/_editable/Artifacts.xlsx
+++ b/doc/_editable/Artifacts.xlsx
@@ -1226,10 +1226,10 @@
   <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C74" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D74" sqref="D74"/>
+      <selection pane="bottomRight" activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Rm some code + notes
</commit_message>
<xml_diff>
--- a/doc/_editable/Artifacts.xlsx
+++ b/doc/_editable/Artifacts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="128">
   <si>
     <t>Notes</t>
   </si>
@@ -400,6 +400,12 @@
   </si>
   <si>
     <t>We tried to use SharePoint the first half of the project, to set up meetings et cetera</t>
+  </si>
+  <si>
+    <t>Mailflow (correspondence)</t>
+  </si>
+  <si>
+    <t>Well over 300 mails!</t>
   </si>
 </sst>
 </file>
@@ -603,17 +609,17 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -920,8 +926,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F110" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A2:F110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F111" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F111"/>
   <tableColumns count="6">
     <tableColumn id="1" name="General Context" dataDxfId="5"/>
     <tableColumn id="2" name="Particular Context" dataDxfId="4"/>
@@ -1223,13 +1229,13 @@
     <tabColor theme="6" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:G172"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C74" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C105" sqref="C105"/>
+      <selection pane="bottomRight" activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1244,10 +1250,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="10"/>
@@ -1915,34 +1921,34 @@
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="23"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="21"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="23"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="21"/>
     </row>
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="23"/>
-      <c r="B51" s="24" t="s">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="23"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="21"/>
     </row>
     <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
@@ -1957,12 +1963,12 @@
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="23"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="23"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="21"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
@@ -2386,17 +2392,17 @@
       <c r="A85" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B85" s="24" t="s">
+      <c r="B85" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="C85" s="24" t="s">
+      <c r="C85" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D85" s="24" t="s">
+      <c r="D85" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="E85" s="24"/>
-      <c r="F85" s="23"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="21"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
@@ -2434,48 +2440,50 @@
       <c r="A88" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D88" s="22"/>
+      <c r="E88" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F88" s="21"/>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C88" s="15" t="s">
+      <c r="C89" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D88" s="15" t="s">
+      <c r="D89" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E88" s="15" t="s">
+      <c r="E89" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F88" s="5"/>
-    </row>
-    <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="15"/>
-      <c r="B89" s="15"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
-      <c r="E89" s="15"/>
       <c r="F89" s="5"/>
     </row>
-    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
-        <v>85</v>
-      </c>
+    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="15"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
       <c r="D90" s="15"/>
       <c r="E90" s="15"/>
       <c r="F90" s="5"/>
     </row>
-    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>88</v>
-      </c>
+    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91" s="15"/>
+      <c r="C91" s="15"/>
       <c r="D91" s="15"/>
       <c r="E91" s="15"/>
       <c r="F91" s="5"/>
@@ -2485,10 +2493,10 @@
         <v>2</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="D92" s="15"/>
       <c r="E92" s="15"/>
@@ -2498,39 +2506,39 @@
       <c r="A93" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B93" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="C93" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D93" s="24"/>
-      <c r="E93" s="24"/>
-      <c r="F93" s="23"/>
+      <c r="B93" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C93" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D93" s="15"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="5"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B94" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D94" s="15"/>
-      <c r="E94" s="15"/>
-      <c r="F94" s="5"/>
+      <c r="B94" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D94" s="22"/>
+      <c r="E94" s="22"/>
+      <c r="F94" s="21"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C95" s="15" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="D95" s="15"/>
       <c r="E95" s="15"/>
@@ -2541,10 +2549,10 @@
         <v>2</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D96" s="15"/>
       <c r="E96" s="15"/>
@@ -2555,10 +2563,10 @@
         <v>2</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="D97" s="15"/>
       <c r="E97" s="15"/>
@@ -2569,15 +2577,13 @@
         <v>2</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C98" s="15" t="s">
         <v>88</v>
       </c>
       <c r="D98" s="15"/>
-      <c r="E98" s="15" t="s">
-        <v>125</v>
-      </c>
+      <c r="E98" s="15"/>
       <c r="F98" s="5"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2585,19 +2591,27 @@
         <v>2</v>
       </c>
       <c r="B99" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C99" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D99" s="15"/>
+      <c r="E99" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F99" s="5"/>
+    </row>
+    <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C99" s="15" t="s">
+      <c r="C100" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D99" s="15"/>
-      <c r="E99" s="15"/>
-      <c r="F99" s="5"/>
-    </row>
-    <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="15"/>
-      <c r="B100" s="15"/>
-      <c r="C100" s="15"/>
       <c r="D100" s="15"/>
       <c r="E100" s="15"/>
       <c r="F100" s="5"/>
@@ -2682,7 +2696,14 @@
       <c r="E110" s="15"/>
       <c r="F110" s="5"/>
     </row>
-    <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="15"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="15"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="5"/>
+    </row>
     <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2743,6 +2764,7 @@
     <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Added User Story descrip docx
</commit_message>
<xml_diff>
--- a/doc/_editable/Artifacts.xlsx
+++ b/doc/_editable/Artifacts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="129">
   <si>
     <t>Notes</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>Well over 300 mails!</t>
+  </si>
+  <si>
+    <t>User Stories Description</t>
   </si>
 </sst>
 </file>
@@ -926,8 +929,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F111" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A2:F111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F112" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F112"/>
   <tableColumns count="6">
     <tableColumn id="1" name="General Context" dataDxfId="5"/>
     <tableColumn id="2" name="Particular Context" dataDxfId="4"/>
@@ -1229,13 +1232,13 @@
     <tabColor theme="6" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G172"/>
+  <dimension ref="A1:G173"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C74" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E88" sqref="E88"/>
+      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2342,90 +2345,88 @@
       <c r="A81" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="15" t="s">
+      <c r="B81" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="21"/>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C81" s="15" t="s">
+      <c r="C82" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="5"/>
-    </row>
-    <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="15"/>
-      <c r="B82" s="15"/>
-      <c r="C82" s="15"/>
       <c r="D82" s="15"/>
       <c r="E82" s="15"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>89</v>
-      </c>
+    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="15"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
       <c r="F83" s="5"/>
     </row>
-    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C84" s="15" t="s">
-        <v>88</v>
-      </c>
+    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" s="15"/>
+      <c r="C84" s="15"/>
       <c r="D84" s="15"/>
-      <c r="E84" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="F84" s="15" t="s">
-        <v>92</v>
-      </c>
+      <c r="E84" s="15"/>
+      <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B85" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C85" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D85" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="E85" s="22"/>
-      <c r="F85" s="21"/>
+      <c r="B85" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F85" s="15" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B86" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D86" s="15"/>
-      <c r="E86" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F86" s="5"/>
+      <c r="B86" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D86" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E86" s="22"/>
+      <c r="F86" s="21"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>88</v>
@@ -2440,64 +2441,66 @@
       <c r="A88" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B88" s="22" t="s">
-        <v>126</v>
+      <c r="B88" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D88" s="22"/>
-      <c r="E88" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="F88" s="21"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D89" s="22"/>
+      <c r="E89" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F89" s="21"/>
+    </row>
+    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C89" s="15" t="s">
+      <c r="C90" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D89" s="15" t="s">
+      <c r="D90" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E89" s="15" t="s">
+      <c r="E90" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F89" s="5"/>
-    </row>
-    <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="15"/>
-      <c r="B90" s="15"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15"/>
       <c r="F90" s="5"/>
     </row>
-    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="17" t="s">
-        <v>85</v>
-      </c>
+    <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="15"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
       <c r="D91" s="15"/>
       <c r="E91" s="15"/>
       <c r="F91" s="5"/>
     </row>
-    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B92" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>88</v>
-      </c>
+    <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" s="15"/>
+      <c r="C92" s="15"/>
       <c r="D92" s="15"/>
       <c r="E92" s="15"/>
       <c r="F92" s="5"/>
@@ -2507,10 +2510,10 @@
         <v>2</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="D93" s="15"/>
       <c r="E93" s="15"/>
@@ -2520,39 +2523,39 @@
       <c r="A94" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B94" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C94" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="21"/>
+      <c r="B94" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D94" s="15"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="5"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B95" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D95" s="15"/>
-      <c r="E95" s="15"/>
-      <c r="F95" s="5"/>
+      <c r="B95" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D95" s="22"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="21"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="D96" s="15"/>
       <c r="E96" s="15"/>
@@ -2563,10 +2566,10 @@
         <v>2</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C97" s="15" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D97" s="15"/>
       <c r="E97" s="15"/>
@@ -2577,10 +2580,10 @@
         <v>2</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="D98" s="15"/>
       <c r="E98" s="15"/>
@@ -2591,15 +2594,13 @@
         <v>2</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C99" s="15" t="s">
         <v>88</v>
       </c>
       <c r="D99" s="15"/>
-      <c r="E99" s="15" t="s">
-        <v>125</v>
-      </c>
+      <c r="E99" s="15"/>
       <c r="F99" s="5"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2607,19 +2608,27 @@
         <v>2</v>
       </c>
       <c r="B100" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D100" s="15"/>
+      <c r="E100" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F100" s="5"/>
+    </row>
+    <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C100" s="15" t="s">
+      <c r="C101" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D100" s="15"/>
-      <c r="E100" s="15"/>
-      <c r="F100" s="5"/>
-    </row>
-    <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="15"/>
-      <c r="B101" s="15"/>
-      <c r="C101" s="15"/>
       <c r="D101" s="15"/>
       <c r="E101" s="15"/>
       <c r="F101" s="5"/>
@@ -2704,7 +2713,14 @@
       <c r="E111" s="15"/>
       <c r="F111" s="5"/>
     </row>
-    <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="15"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="15"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="5"/>
+    </row>
     <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2765,6 +2781,7 @@
     <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
Loads of updated documents and other
</commit_message>
<xml_diff>
--- a/doc/_editable/Artifacts.xlsx
+++ b/doc/_editable/Artifacts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7110"/>
   </bookViews>
   <sheets>
     <sheet name="MyBar Artifacts" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'MyBar Artifacts'!$A$1:$E$59</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="131">
   <si>
     <t>Notes</t>
   </si>
@@ -203,9 +203,6 @@
     <t>view_drink.xml</t>
   </si>
   <si>
-    <t>Adam Clark, Viktor Edsand</t>
-  </si>
-  <si>
     <t>view_settings.xml</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>Description and Features</t>
   </si>
   <si>
-    <t>Development Introduction</t>
-  </si>
-  <si>
     <t>Known Bugs and Limitations</t>
   </si>
   <si>
@@ -401,9 +395,6 @@
     <t>Mathias Bjurbäck, Viktor Edsand, Dag Fridén, Mathias Karlgren</t>
   </si>
   <si>
-    <t>Viktor Edsand, Mathias Karlgren</t>
-  </si>
-  <si>
     <t>User Stories Description</t>
   </si>
   <si>
@@ -411,13 +402,31 @@
   </si>
   <si>
     <t>Mathias Karlgren, Viktor Edsand</t>
+  </si>
+  <si>
+    <t>Development Manual</t>
+  </si>
+  <si>
+    <t>Adam Clark, Mathias Karlgren, Viktor Edsand</t>
+  </si>
+  <si>
+    <t>UPPDATERA UML</t>
+  </si>
+  <si>
+    <t>SKRIV KLART ADAM</t>
+  </si>
+  <si>
+    <t>Reflection</t>
+  </si>
+  <si>
+    <t>Adam Clark, Mathias Bjurbäck, Mathias Karlgren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -468,6 +477,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -475,12 +485,21 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -567,7 +586,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -623,6 +642,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -938,8 +967,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F113" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A2:F113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F114" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F114"/>
   <tableColumns count="6">
     <tableColumn id="1" name="General Context" dataDxfId="5"/>
     <tableColumn id="2" name="Particular Context" dataDxfId="4"/>
@@ -1241,13 +1270,13 @@
     <tabColor theme="6" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G173"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C61" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C63" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1255,17 +1284,17 @@
     <col min="1" max="1" width="39.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="66.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" style="4" customWidth="1"/>
     <col min="5" max="5" width="79" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="10"/>
@@ -1273,10 +1302,10 @@
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>40</v>
@@ -1288,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -1891,7 +1920,7 @@
         <v>2</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>39</v>
@@ -1905,7 +1934,7 @@
         <v>2</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>43</v>
@@ -1922,7 +1951,7 @@
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
@@ -1933,7 +1962,7 @@
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="19"/>
       <c r="B50" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>44</v>
@@ -1945,10 +1974,10 @@
     <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
       <c r="B51" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
@@ -1964,7 +1993,7 @@
     </row>
     <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -1977,14 +2006,14 @@
         <v>2</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>42</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F54" s="5"/>
     </row>
@@ -1993,7 +2022,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>46</v>
@@ -2012,7 +2041,7 @@
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
@@ -2076,7 +2105,7 @@
     </row>
     <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
@@ -2089,10 +2118,10 @@
         <v>2</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D63" s="15"/>
       <c r="E63" s="15"/>
@@ -2103,10 +2132,10 @@
         <v>2</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
@@ -2117,12 +2146,14 @@
         <v>2</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D65" s="15"/>
+      <c r="D65" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="E65" s="15"/>
       <c r="F65" s="5"/>
     </row>
@@ -2131,12 +2162,14 @@
         <v>2</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D66" s="15"/>
+      <c r="D66" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="E66" s="15"/>
       <c r="F66" s="5"/>
     </row>
@@ -2145,7 +2178,7 @@
         <v>2</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>39</v>
@@ -2159,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>42</v>
@@ -2173,7 +2206,7 @@
         <v>2</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C69" s="15" t="s">
         <v>39</v>
@@ -2187,12 +2220,14 @@
         <v>2</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D70" s="15"/>
+      <c r="D70" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="E70" s="15"/>
       <c r="F70" s="5"/>
     </row>
@@ -2201,12 +2236,14 @@
         <v>2</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C71" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D71" s="15"/>
+      <c r="D71" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="E71" s="15"/>
       <c r="F71" s="5"/>
     </row>
@@ -2215,12 +2252,14 @@
         <v>2</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D72" s="15"/>
+      <c r="D72" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="E72" s="15"/>
       <c r="F72" s="5"/>
     </row>
@@ -2229,7 +2268,7 @@
         <v>2</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C73" s="15" t="s">
         <v>45</v>
@@ -2243,7 +2282,7 @@
         <v>2</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>42</v>
@@ -2257,13 +2296,13 @@
         <v>2</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E75" s="15"/>
       <c r="F75" s="5"/>
@@ -2273,7 +2312,7 @@
         <v>2</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>43</v>
@@ -2287,15 +2326,13 @@
         <v>2</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="D77" s="15"/>
-      <c r="E77" s="15" t="s">
-        <v>102</v>
-      </c>
+      <c r="E77" s="15"/>
       <c r="F77" s="5"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2303,13 +2340,15 @@
         <v>2</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D78" s="15"/>
-      <c r="E78" s="15"/>
+      <c r="E78" s="15" t="s">
+        <v>100</v>
+      </c>
       <c r="F78" s="5"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2317,13 +2356,15 @@
         <v>2</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D79" s="15"/>
-      <c r="E79" s="15"/>
+      <c r="E79" s="15" t="s">
+        <v>127</v>
+      </c>
       <c r="F79" s="5"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2331,111 +2372,113 @@
         <v>2</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C80" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D80" s="15"/>
+      <c r="E80" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="19"/>
-    </row>
-    <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B81" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="5"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="23"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="15"/>
-      <c r="B82" s="15"/>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
+      <c r="A82" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>43</v>
+      </c>
       <c r="E82" s="15"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>82</v>
-      </c>
+    <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="15"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
       <c r="F83" s="5"/>
     </row>
-    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C84" s="15" t="s">
-        <v>81</v>
-      </c>
+    <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B84" s="15"/>
+      <c r="C84" s="15"/>
       <c r="D84" s="15"/>
-      <c r="E84" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F84" s="15" t="s">
-        <v>84</v>
-      </c>
+      <c r="E84" s="15"/>
+      <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C85" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D85" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E85" s="20"/>
-      <c r="F85" s="19"/>
+        <v>117</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F85" s="15" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D86" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C86" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E86" s="15"/>
-      <c r="F86" s="5"/>
+      <c r="D86" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E86" s="20"/>
+      <c r="F86" s="19"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D87" s="15"/>
-      <c r="E87" s="15" t="s">
-        <v>91</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E87" s="15"/>
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2443,14 +2486,14 @@
         <v>2</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="D88" s="15"/>
       <c r="E88" s="15" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="F88" s="5"/>
     </row>
@@ -2459,14 +2502,14 @@
         <v>2</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="D89" s="15"/>
       <c r="E89" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F89" s="5"/>
     </row>
@@ -2475,14 +2518,14 @@
         <v>2</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="C90" s="15" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="D90" s="15"/>
       <c r="E90" s="15" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="F90" s="5"/>
     </row>
@@ -2490,64 +2533,66 @@
       <c r="A91" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B91" s="20" t="s">
-        <v>109</v>
+      <c r="B91" s="15" t="s">
+        <v>85</v>
       </c>
       <c r="C91" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F91" s="19"/>
+        <v>79</v>
+      </c>
+      <c r="D91" s="15"/>
+      <c r="E91" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F91" s="5"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B92" s="15" t="s">
-        <v>90</v>
+      <c r="B92" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="C92" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D92" s="20"/>
+      <c r="E92" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F92" s="19"/>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D92" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E92" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F92" s="5"/>
-    </row>
-    <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="15"/>
-      <c r="B93" s="15"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="15"/>
+      <c r="C93" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E93" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="F93" s="5"/>
     </row>
-    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
-        <v>78</v>
-      </c>
+    <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="15"/>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
       <c r="D94" s="15"/>
       <c r="E94" s="15"/>
       <c r="F94" s="5"/>
     </row>
-    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B95" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>81</v>
-      </c>
+    <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B95" s="15"/>
+      <c r="C95" s="15"/>
       <c r="D95" s="15"/>
       <c r="E95" s="15"/>
       <c r="F95" s="5"/>
@@ -2557,10 +2602,10 @@
         <v>2</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="D96" s="15"/>
       <c r="E96" s="15"/>
@@ -2570,39 +2615,39 @@
       <c r="A97" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B97" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C97" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D97" s="20"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="19"/>
+      <c r="B97" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="5"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B98" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D98" s="15"/>
-      <c r="E98" s="15"/>
-      <c r="F98" s="5"/>
+      <c r="B98" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C98" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="19"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="D99" s="15"/>
       <c r="E99" s="15"/>
@@ -2613,10 +2658,10 @@
         <v>2</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C100" s="15" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="D100" s="15"/>
       <c r="E100" s="15"/>
@@ -2627,15 +2672,13 @@
         <v>2</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D101" s="15"/>
-      <c r="E101" s="15" t="s">
-        <v>126</v>
-      </c>
+      <c r="E101" s="15"/>
       <c r="F101" s="5"/>
     </row>
     <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2643,19 +2686,27 @@
         <v>2</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C102" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D102" s="15"/>
+      <c r="E102" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F102" s="5"/>
+    </row>
+    <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D102" s="15"/>
-      <c r="E102" s="15"/>
-      <c r="F102" s="5"/>
-    </row>
-    <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="15"/>
-      <c r="B103" s="15"/>
-      <c r="C103" s="15"/>
+      <c r="C103" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="D103" s="15"/>
       <c r="E103" s="15"/>
       <c r="F103" s="5"/>
@@ -2740,7 +2791,14 @@
       <c r="E113" s="15"/>
       <c r="F113" s="5"/>
     </row>
-    <row r="114" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="15"/>
+      <c r="B114" s="15"/>
+      <c r="C114" s="15"/>
+      <c r="D114" s="15"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="5"/>
+    </row>
     <row r="115" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="116" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="117" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2800,6 +2858,7 @@
     <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>